<commit_message>
Second set of updates for HU
-loads initial and tax donor populations
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="9">
   <si>
     <t>Country</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>2019</t>
+  </si>
+  <si>
+    <t>HU</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working version of PL model
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="10">
   <si>
     <t>Country</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>HU</t>
+  </si>
+  <si>
+    <t>PL</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Update population projections. Add liwwh var.
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="10">
   <si>
     <t>Country</t>
   </si>
@@ -434,7 +434,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 00_master.do to reflect new wave of UKHLS
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>